<commit_message>
Add Mail WF and Change Process WF Structure
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -272,17 +272,27 @@
   </si>
   <si>
     <t>OutputFolderDirectory</t>
+  </si>
+  <si>
+    <t>ExcelFileSchema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -376,27 +386,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +626,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -740,7 +751,7 @@
       </c>
       <c r="B13" s="7" t="str">
         <f ca="1">CONCATENATE("Daily Onboarding Process Report -(",TEXT(NOW(),"yyyy/mm/dd"),")")</f>
-        <v>Daily Onboarding Process Report -(2025/11/23)</v>
+        <v>Daily Onboarding Process Report -(2025/11/25)</v>
       </c>
       <c r="C13" s="17"/>
     </row>
@@ -794,7 +805,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="str">
+        <f ca="1">CONCATENATE("Onboarding_Report_",TEXT(NOW(),"yyyy-mm-dd"),".xlsx")</f>
+        <v>Onboarding_Report_2025-11-25.xlsx</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>